<commit_message>
YSI batch prediction of monoterpenes
YSI batch prediction of monoterpenes based on cactus API, YSI database access on 01/01/2022 (Happy New Year!)
</commit_message>
<xml_diff>
--- a/YSI results.xlsx
+++ b/YSI results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>SMILES</t>
@@ -441,185 +446,481 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>CAS</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CAS</t>
+          <t>measured YSI</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>measured YSI</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>predicted YSI</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>R-limonene</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C=C(C)[C@H]1CC=C(C)CC1</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>0-0-0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>137.1057140728124</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>limonane</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[N-]=[N+]=O</t>
+          <t>CC1CCC(C(C)C)CC1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10024-97-2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>89.56030102639519</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sabinene</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CCC(C)C</t>
+          <t>C=C1CCC2(C(C)C)CC12</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>78-78-4</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="n">
-        <v>30.65434248076865</v>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dihydrosabinene</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CC(C)=O</t>
+          <t>CC1CCC2(C(C)C)CC12</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>67-64-1</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>13</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6.289965615761659</v>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tetrahydrosabinene</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CCCC(C)C</t>
+          <t>CC1CCC(C1)(C)C(C)C</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>107-83-5</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>36.7</v>
-      </c>
-      <c r="F6" t="n">
-        <v>37.09619135574087</v>
+        <v>96.28969729646181</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>α-pinene</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CCC(C)CC</t>
+          <t>CC1=CCC2CC1C2(C)C</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>96-14-0</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>38.2</v>
-      </c>
-      <c r="F7" t="n">
-        <v>37.09619135574087</v>
+        <v>149.6251082802425</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>β-pinene</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CCCCCC</t>
+          <t>CC1(C)C2CCC(C1C2)=C</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>110-54-3</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>30.4</v>
-      </c>
-      <c r="F8" t="n">
-        <v>31.38920766898859</v>
+        <v>141.7593009049891</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>pinane</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CC1CCCC1</t>
+          <t>CC1CCC2CC1C2(C)C</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>96-37-7</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>50.3</v>
-      </c>
-      <c r="F9" t="n">
-        <v>50.42235746787229</v>
+        <v>112.7067722234206</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3-carene</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CC1=CCC2C(C1)C2(C)C</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dihydrocarene</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CC1CCC2C(C1)C2(C)C</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>tetrahydrocarene</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CC1CCCC(C)(C)CC1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>92.73422083809098</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1,4-dimethylcyclooctane</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CC1CCCCC(C)CC1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>86.00482456802436</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1,8-cineole</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CC1(C2CCC(O1)(CC2)C)C</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>101.5425511215314</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1,4-cineole</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CC(C)C12CCC(O1)(CC2)C</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>99.10287317265235</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>S-carvone</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CC1=CC[C@@H](CC1=O)C(=C)C</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>R-carvone</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CC1=CC[C@H](CC1=O)C(=C)C </t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>outlier</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>myrcene</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CC(=CCCC(=C)C=C)C</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>84.17913766113249</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>β-ocimene</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CC(=CCC=C(C)C=C)C</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>89.64658374609849</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>dihydromyrcene</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CC(C=C)CC/C=C(C)\C</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>93.6933830544498</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>farnesane</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CCC(C)CCCC(C)CCCC(C)C</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>109.8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>106.7640468372568</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>geranial</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CC(=CCCC(=CC=O)C)C</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>86.43653279452629</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>geraniol</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CC(=CCCC(=CCO)C)C</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>101.3285698974017</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>citronellal</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CC(CCC=C(C)C)CC=O</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
+        <v>77.47969437084743</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>carvacrol</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CC1=C(C=C(C=C1)C(C)C)O</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>253.3179781004491</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>linalool</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CC(=CCCC(C)(C=C)O)C</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>91.14313433953583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>